<commit_message>
fixed logic bug in findtriangle and plotted graph
</commit_message>
<xml_diff>
--- a/cs101_hwk1.xlsx
+++ b/cs101_hwk1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinmintz17/Desktop/CSE 101/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thinmintz17/Desktop/CSE 101/findTriangle/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>n</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>Testing Random graph</t>
+  </si>
+  <si>
+    <t>time bp</t>
+  </si>
+  <si>
+    <t>logbptime</t>
   </si>
 </sst>
 </file>
@@ -58,7 +64,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF00F900"/>
       <name val="Menlo"/>
       <family val="2"/>
     </font>
@@ -85,11 +91,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -139,8 +145,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>random graph bench mark</a:t>
+              <a:t>Benchmarking</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Algorithm</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -183,6 +194,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>random_graphs</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="31750" cap="rnd">
               <a:noFill/>
@@ -205,6 +219,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.0548177600321206"/>
+                  <c:y val="0.0828893383916867"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$11</c:f>
@@ -248,31 +312,183 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-10.99291629402088</c:v>
+                  <c:v>-9.879111703025005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-10.0520954491453</c:v>
+                  <c:v>-9.761747574027575</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.07119012920761</c:v>
+                  <c:v>-8.673414851728955</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.768234535555082</c:v>
+                  <c:v>-7.859911230220318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-6.726033882606757</c:v>
+                  <c:v>-6.76740380796966</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.318745604346663</c:v>
+                  <c:v>-5.23932308337971</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.899665431582989</c:v>
+                  <c:v>-3.88129372547754</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.353738395282</c:v>
+                  <c:v>-2.19608250951901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.684728218060912</c:v>
+                  <c:v>-0.561746762469954</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>bipartite</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0407063192879927"/>
+                  <c:y val="0.0373051246212746"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$3:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.386294361119891</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.079441541679836</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.772588722239781</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.465735902799727</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.158883083359671</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.852030263919617</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.545177444479562</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.238324625039507</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6.954638864880987</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$3:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-9.666870119552795</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-7.963457300986761</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-6.858719732730874</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.161106561619385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-3.916937903436088</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-2.52858710284224</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.124306025024616</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.329804016274898</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.861023736547825</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -287,11 +503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1513074320"/>
-        <c:axId val="-1513076640"/>
+        <c:axId val="1045481440"/>
+        <c:axId val="1045484992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1513074320"/>
+        <c:axId val="1045481440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,12 +563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1513076640"/>
+        <c:crossAx val="1045484992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1513076640"/>
+        <c:axId val="1045484992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -372,6 +588,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -408,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1513074320"/>
+        <c:crossAx val="1045481440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -420,6 +637,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1017,20 +1266,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1311,10 +1560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,15 +1571,15 @@
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1343,13 +1592,19 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>1.6820430755600001E-5</v>
+      <c r="B3" s="2">
+        <v>5.12337684631E-5</v>
       </c>
       <c r="C3">
         <f>LN(A3:A11)</f>
@@ -1357,15 +1612,22 @@
       </c>
       <c r="D3">
         <f>LN(B3)</f>
-        <v>-10.99291629402088</v>
+        <v>-9.8791117030250053</v>
+      </c>
+      <c r="E3" s="2">
+        <v>6.3347816467299994E-5</v>
+      </c>
+      <c r="F3">
+        <f>LN(E3)</f>
+        <v>-9.6668701195527955</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
-        <v>4.3095350265500001E-5</v>
+      <c r="B4" s="2">
+        <v>5.7613849639899999E-5</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C11" si="0">LN(A4:A12)</f>
@@ -1373,15 +1635,22 @@
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D11" si="1">LN(B4)</f>
-        <v>-10.052095449145302</v>
+        <v>-9.7617475740275754</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3.4794807434099999E-4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F11" si="2">LN(E4)</f>
+        <v>-7.9634573009867609</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
-        <v>1.14929676056E-4</v>
+      <c r="B5" s="3">
+        <v>1.71073913574E-4</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -1389,15 +1658,22 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-9.0711901292076096</v>
+        <v>-8.6734148517289551</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0502576828000001E-3</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>-6.8587197327308749</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>32</v>
       </c>
-      <c r="B6" s="2">
-        <v>4.2295932769800002E-4</v>
+      <c r="B6" s="3">
+        <v>3.8590812683099999E-4</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -1405,15 +1681,22 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>-7.7682345355550817</v>
+        <v>-7.8599112302203178</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.7353496551500001E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="2"/>
+        <v>-5.161106561619385</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>64</v>
       </c>
-      <c r="B7" s="2">
-        <v>1.19928002357E-3</v>
+      <c r="B7" s="3">
+        <v>1.1506781578099999E-3</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -1421,15 +1704,22 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>-6.7260338826067567</v>
+        <v>-6.7674038079696599</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.9901943206799999E-2</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>-3.9169379034360885</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>128</v>
       </c>
-      <c r="B8" s="2">
-        <v>4.8988950252500003E-3</v>
+      <c r="B8" s="3">
+        <v>5.3038458824199997E-3</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -1437,15 +1727,22 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>-5.3187456043466632</v>
+        <v>-5.2393230833797091</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7.97716498375E-2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>-2.5285871028422391</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>256</v>
       </c>
-      <c r="B9" s="2">
-        <v>2.0248684883099999E-2</v>
+      <c r="B9" s="3">
+        <v>2.06241259575E-2</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -1453,15 +1750,22 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>-3.8996654315829891</v>
+        <v>-3.8812937254775393</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.32487784624100002</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="2"/>
+        <v>-1.1243060250246164</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>512</v>
       </c>
-      <c r="B10" s="2">
-        <v>9.5013300180399995E-2</v>
+      <c r="B10" s="3">
+        <v>0.11123808002500001</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -1469,15 +1773,22 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>-2.3537383952820004</v>
+        <v>-2.1960825095190097</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.3906955480600001</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>0.32980401627489825</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1048</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.50422725081399999</v>
+      <c r="B11" s="3">
+        <v>0.57021216821700005</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -1485,7 +1796,14 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>-0.68472821806091255</v>
+        <v>-0.5617467624699537</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6.4303163528400002</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="2"/>
+        <v>1.8610237365478255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I dont know what changes were made
</commit_message>
<xml_diff>
--- a/cs101_hwk1.xlsx
+++ b/cs101_hwk1.xlsx
@@ -91,11 +91,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,11 +503,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1045481440"/>
-        <c:axId val="1045484992"/>
+        <c:axId val="1042427376"/>
+        <c:axId val="1042290944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1045481440"/>
+        <c:axId val="1042427376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,12 +563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1045484992"/>
+        <c:crossAx val="1042290944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1045484992"/>
+        <c:axId val="1042290944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1045481440"/>
+        <c:crossAx val="1042427376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1266,16 +1266,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1563,7 +1563,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1572,12 +1572,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -1603,7 +1603,7 @@
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>5.12337684631E-5</v>
       </c>
       <c r="C3">
@@ -1614,7 +1614,7 @@
         <f>LN(B3)</f>
         <v>-9.8791117030250053</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>6.3347816467299994E-5</v>
       </c>
       <c r="F3">
@@ -1626,7 +1626,7 @@
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>5.7613849639899999E-5</v>
       </c>
       <c r="C4">
@@ -1637,7 +1637,7 @@
         <f t="shared" ref="D4:D11" si="1">LN(B4)</f>
         <v>-9.7617475740275754</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>3.4794807434099999E-4</v>
       </c>
       <c r="F4">
@@ -1649,7 +1649,7 @@
       <c r="A5">
         <v>16</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1.71073913574E-4</v>
       </c>
       <c r="C5">
@@ -1660,7 +1660,7 @@
         <f t="shared" si="1"/>
         <v>-8.6734148517289551</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>1.0502576828000001E-3</v>
       </c>
       <c r="F5">
@@ -1672,7 +1672,7 @@
       <c r="A6">
         <v>32</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>3.8590812683099999E-4</v>
       </c>
       <c r="C6">
@@ -1683,7 +1683,7 @@
         <f t="shared" si="1"/>
         <v>-7.8599112302203178</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <v>5.7353496551500001E-3</v>
       </c>
       <c r="F6">
@@ -1695,7 +1695,7 @@
       <c r="A7">
         <v>64</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>1.1506781578099999E-3</v>
       </c>
       <c r="C7">
@@ -1706,7 +1706,7 @@
         <f t="shared" si="1"/>
         <v>-6.7674038079696599</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>1.9901943206799999E-2</v>
       </c>
       <c r="F7">
@@ -1718,7 +1718,7 @@
       <c r="A8">
         <v>128</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>5.3038458824199997E-3</v>
       </c>
       <c r="C8">
@@ -1729,7 +1729,7 @@
         <f t="shared" si="1"/>
         <v>-5.2393230833797091</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>7.97716498375E-2</v>
       </c>
       <c r="F8">
@@ -1741,7 +1741,7 @@
       <c r="A9">
         <v>256</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>2.06241259575E-2</v>
       </c>
       <c r="C9">
@@ -1752,7 +1752,7 @@
         <f t="shared" si="1"/>
         <v>-3.8812937254775393</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>0.32487784624100002</v>
       </c>
       <c r="F9">
@@ -1764,7 +1764,7 @@
       <c r="A10">
         <v>512</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>0.11123808002500001</v>
       </c>
       <c r="C10">
@@ -1775,7 +1775,7 @@
         <f t="shared" si="1"/>
         <v>-2.1960825095190097</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1.3906955480600001</v>
       </c>
       <c r="F10">
@@ -1787,7 +1787,7 @@
       <c r="A11">
         <v>1048</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>0.57021216821700005</v>
       </c>
       <c r="C11">
@@ -1798,7 +1798,7 @@
         <f t="shared" si="1"/>
         <v>-0.5617467624699537</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>6.4303163528400002</v>
       </c>
       <c r="F11">

</xml_diff>

<commit_message>
finished experiment and doing writeup
</commit_message>
<xml_diff>
--- a/cs101_hwk1.xlsx
+++ b/cs101_hwk1.xlsx
@@ -89,13 +89,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -235,8 +236,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0548177600321206"/>
-                  <c:y val="0.0828893383916867"/>
+                  <c:x val="-0.0821704847092414"/>
+                  <c:y val="-0.00155275243295801"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -271,36 +272,36 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$11</c:f>
+              <c:f>Sheet1!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.386294361119891</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.079441541679836</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.772588722239781</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.465735902799727</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.158883083359671</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.852030263919617</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.545177444479562</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.238324625039507</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.954638864880987</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -312,31 +313,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-9.879111703025005</c:v>
+                  <c:v>-4.966289727298272</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-9.761747574027575</c:v>
+                  <c:v>-4.452899741807043</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-8.673414851728955</c:v>
+                  <c:v>-4.179741045105715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-7.859911230220318</c:v>
+                  <c:v>-3.760624762851438</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-6.76740380796966</c:v>
+                  <c:v>-3.262441813896901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.23932308337971</c:v>
+                  <c:v>-2.751700600255472</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-3.88129372547754</c:v>
+                  <c:v>-2.282441308426479</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-2.19608250951901</c:v>
+                  <c:v>-1.747782203753706</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.561746762469954</c:v>
+                  <c:v>-1.208337958340171</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -387,8 +388,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.0407063192879927"/>
-                  <c:y val="0.0373051246212746"/>
+                  <c:x val="-0.0127653855590997"/>
+                  <c:y val="0.148996866020193"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -423,36 +424,36 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$11</c:f>
+              <c:f>Sheet1!$B$3:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.386294361119891</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.079441541679836</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.772588722239781</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.465735902799727</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.158883083359671</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.852030263919617</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.545177444479562</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.238324625039507</c:v>
+                  <c:v>9.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.954638864880987</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -464,31 +465,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-9.666870119552795</c:v>
+                  <c:v>-20.64950275291583</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.963457300986761</c:v>
+                  <c:v>-19.29956028185905</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.858719732730874</c:v>
+                  <c:v>-17.98653774019353</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5.161106561619385</c:v>
+                  <c:v>-16.35903208954622</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.916937903436088</c:v>
+                  <c:v>-13.91598890154516</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-2.52858710284224</c:v>
+                  <c:v>-11.90638436751189</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-1.124306025024616</c:v>
+                  <c:v>-10.08718549429133</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.329804016274898</c:v>
+                  <c:v>-7.721307354325705</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.861023736547825</c:v>
+                  <c:v>-5.464450468105252</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -503,11 +504,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1042427376"/>
-        <c:axId val="1042290944"/>
+        <c:axId val="1048417872"/>
+        <c:axId val="1000698224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1042427376"/>
+        <c:axId val="1048417872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -527,6 +528,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log(|V|)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -563,12 +620,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1042290944"/>
+        <c:crossAx val="1000698224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1042290944"/>
+        <c:axId val="1000698224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,6 +645,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log(runtime)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -625,7 +738,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1042427376"/>
+        <c:crossAx val="1048417872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1266,16 +1379,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1560,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1584,10 +1697,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1603,207 +1716,230 @@
       <c r="A3">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>5.12337684631E-5</v>
-      </c>
-      <c r="C3">
-        <f>LN(A3:A11)</f>
-        <v>1.3862943611198906</v>
+      <c r="B3">
+        <f>LOG(A3, 2)</f>
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>3.4570693969700002E-7</v>
       </c>
       <c r="D3">
-        <f>LN(B3)</f>
-        <v>-9.8791117030250053</v>
+        <f>LOG(C3, 20)</f>
+        <v>-4.966289727298272</v>
       </c>
       <c r="E3" s="1">
-        <v>6.3347816467299994E-5</v>
+        <v>6.07967376709E-7</v>
       </c>
       <c r="F3">
-        <f>LN(E3)</f>
-        <v>-9.6668701195527955</v>
+        <f>LOG(E3, 2)</f>
+        <v>-20.649502752915829</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8</v>
       </c>
-      <c r="B4" s="1">
-        <v>5.7613849639899999E-5</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C11" si="0">LN(A4:A12)</f>
-        <v>2.0794415416798357</v>
+      <c r="B4">
+        <f t="shared" ref="B4:B12" si="0">LOG(A4, 2)</f>
+        <v>3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.6093254089399999E-6</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D11" si="1">LN(B4)</f>
-        <v>-9.7617475740275754</v>
-      </c>
-      <c r="E4" s="2">
-        <v>3.4794807434099999E-4</v>
+        <f t="shared" ref="D4:D12" si="1">LOG(C4, 20)</f>
+        <v>-4.4528997418070428</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1.54972076416E-6</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F11" si="2">LN(E4)</f>
-        <v>-7.9634573009867609</v>
+        <f t="shared" ref="F4:F12" si="2">LOG(E4, 2)</f>
+        <v>-19.299560281859051</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>16</v>
       </c>
-      <c r="B5" s="2">
-        <v>1.71073913574E-4</v>
-      </c>
-      <c r="C5">
+      <c r="B5">
         <f t="shared" si="0"/>
-        <v>2.7725887222397811</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="4">
+        <v>3.6478042602499999E-6</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-8.6734148517289551</v>
-      </c>
-      <c r="E5" s="2">
-        <v>1.0502576828000001E-3</v>
+        <v>-4.1797410451057155</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3.8504600524900003E-6</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>-6.8587197327308749</v>
+        <v>-17.986537740193526</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>32</v>
       </c>
-      <c r="B6" s="2">
-        <v>3.8590812683099999E-4</v>
-      </c>
-      <c r="C6">
+      <c r="B6">
         <f t="shared" si="0"/>
-        <v>3.4657359027997265</v>
+        <v>5</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1.2803077697800001E-5</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>-7.8599112302203178</v>
-      </c>
-      <c r="E6" s="2">
-        <v>5.7353496551500001E-3</v>
+        <v>-3.7606247628514384</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.18970870972E-5</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>-5.161106561619385</v>
+        <v>-16.359032089546218</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>64</v>
       </c>
-      <c r="B7" s="2">
-        <v>1.1506781578099999E-3</v>
-      </c>
-      <c r="C7">
+      <c r="B7">
         <f t="shared" si="0"/>
-        <v>4.1588830833596715</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>5.6946277618400002E-5</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>-6.7674038079696599</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1.9901943206799999E-2</v>
+        <v>-3.2624418138969014</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.4694881439200004E-5</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>-3.9169379034360885</v>
+        <v>-13.915988901545164</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>128</v>
       </c>
-      <c r="B8" s="2">
-        <v>5.3038458824199997E-3</v>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>4.8520302639196169</v>
+        <v>2.6299953460699998E-4</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>-5.2393230833797091</v>
+        <v>-2.7517006002554725</v>
       </c>
       <c r="E8" s="2">
-        <v>7.97716498375E-2</v>
+        <v>2.6050806045500001E-4</v>
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>-2.5285871028422391</v>
+        <v>-11.906384367511889</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>256</v>
       </c>
-      <c r="B9" s="2">
-        <v>2.06241259575E-2</v>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>5.5451774444795623</v>
+        <v>1.0726928710899999E-3</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>-3.8812937254775393</v>
+        <v>-2.282441308426479</v>
       </c>
       <c r="E9" s="2">
-        <v>0.32487784624100002</v>
+        <v>9.192943573E-4</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>-1.1243060250246164</v>
+        <v>-10.087185494291335</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>512</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.11123808002500001</v>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>6.2383246250395077</v>
+        <v>5.3220987319899998E-3</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>-2.1960825095190097</v>
+        <v>-1.7477822037537063</v>
       </c>
       <c r="E10" s="2">
-        <v>1.3906955480600001</v>
+        <v>4.7386527061499999E-3</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>0.32980401627489825</v>
+        <v>-7.7213073543257051</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1048</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.57021216821700005</v>
+        <v>1024</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>6.9546388648809874</v>
+        <v>2.6786506176000001E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>-0.5617467624699537</v>
+        <v>-1.2083379583401712</v>
       </c>
       <c r="E11" s="2">
-        <v>6.4303163528400002</v>
+        <v>2.2648346424100001E-2</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>1.8610237365478255</v>
+        <v>-5.4644504681052517</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2048</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.14947650432599999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>-0.63444122726854635</v>
+      </c>
+      <c r="E12">
+        <v>0.107604503632</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>-3.2161896337996891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>